<commit_message>
Update naming to be more consistent
</commit_message>
<xml_diff>
--- a/Stackoverflow Threads (Thematic Analysis).xlsx
+++ b/Stackoverflow Threads (Thematic Analysis).xlsx
@@ -5,10 +5,10 @@
   <sheets>
     <sheet state="visible" name="Query" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="All Stackoverflow URL gathered" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Technical" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Codes &amp; Themes for Technical" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Practical" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Codes &amp; Themes for Practical" sheetId="4" r:id="rId7"/>
     <sheet state="visible" name="Debate Answers" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="DAnswers" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="Debate Answers Mean Rank" sheetId="6" r:id="rId9"/>
     <sheet state="visible" name="Codes &amp; Themes for Debate Answe" sheetId="7" r:id="rId10"/>
     <sheet state="visible" name="Debate Questions" sheetId="8" r:id="rId11"/>
     <sheet state="visible" name="Codes &amp; Themes for Debate Quest" sheetId="9" r:id="rId12"/>
@@ -51,7 +51,7 @@
     <t>https://api.stackexchange.com/2.3/search/advanced?pagesize=25&amp;order=desc&amp;sort=relevance&amp;q=test%20private%20method&amp;tagged=unit-testing&amp;site=stackoverflow</t>
   </si>
   <si>
-    <t>test private method U test protected method U test non-public method U test package-private method</t>
+    <t>ALL NON_DUPLICATED LINKS</t>
   </si>
   <si>
     <t>IS IN DEBATE</t>
@@ -554,7 +554,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="32">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -703,18 +703,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="9.0"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="9.0"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -783,18 +771,13 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="62">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -884,9 +867,6 @@
     <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -915,22 +895,16 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="32" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
@@ -950,7 +924,7 @@
     <xf borderId="0" fillId="2" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="33" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1396,7 +1370,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="34.75"/>
-    <col customWidth="1" min="2" max="2" width="19.38"/>
+    <col customWidth="1" min="2" max="2" width="12.88"/>
     <col customWidth="1" min="3" max="3" width="16.38"/>
     <col customWidth="1" min="4" max="4" width="68.13"/>
     <col customWidth="1" min="5" max="6" width="16.38"/>
@@ -1419,11 +1393,11 @@
         <v>13</v>
       </c>
       <c r="B2" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A2)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A2)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C2" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A2)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A2)&gt;0</f>
         <v>1</v>
       </c>
       <c r="G2" s="17"/>
@@ -1434,11 +1408,11 @@
         <v>14</v>
       </c>
       <c r="B3" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A3)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A3)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C3" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A3)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A3)&gt;0</f>
         <v>1</v>
       </c>
       <c r="G3" s="19"/>
@@ -1449,11 +1423,11 @@
         <v>15</v>
       </c>
       <c r="B4" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A4)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A4)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C4" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A4)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A4)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D4" s="21"/>
@@ -1463,11 +1437,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A5)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A5)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C5" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A5)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A5)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D5" s="21"/>
@@ -1477,11 +1451,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A6)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A6)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C6" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A6)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A6)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D6" s="21"/>
@@ -1491,11 +1465,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A7)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A7)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C7" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A7)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A7)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D7" s="21"/>
@@ -1505,11 +1479,11 @@
         <v>19</v>
       </c>
       <c r="B8" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A8)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A8)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C8" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A8)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A8)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D8" s="21"/>
@@ -1519,11 +1493,11 @@
         <v>20</v>
       </c>
       <c r="B9" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A9)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A9)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C9" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A9)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A9)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D9" s="21"/>
@@ -1533,11 +1507,11 @@
         <v>21</v>
       </c>
       <c r="B10" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A10)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A10)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C10" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A10)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A10)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D10" s="21"/>
@@ -1547,11 +1521,11 @@
         <v>22</v>
       </c>
       <c r="B11" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A11)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A11)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C11" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A11)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A11)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D11" s="21"/>
@@ -1561,11 +1535,11 @@
         <v>23</v>
       </c>
       <c r="B12" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A12)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A12)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C12" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A12)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A12)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D12" s="21"/>
@@ -1575,11 +1549,11 @@
         <v>24</v>
       </c>
       <c r="B13" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A13)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A13)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C13" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A13)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A13)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D13" s="21"/>
@@ -1589,11 +1563,11 @@
         <v>25</v>
       </c>
       <c r="B14" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A14)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A14)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C14" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A14)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A14)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D14" s="21"/>
@@ -1603,11 +1577,11 @@
         <v>26</v>
       </c>
       <c r="B15" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A15)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A15)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C15" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A15)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A15)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D15" s="22"/>
@@ -1617,11 +1591,11 @@
         <v>27</v>
       </c>
       <c r="B16" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A16)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A16)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C16" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A16)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A16)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D16" s="22"/>
@@ -1631,11 +1605,11 @@
         <v>28</v>
       </c>
       <c r="B17" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A17)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A17)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C17" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A17)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A17)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D17" s="22"/>
@@ -1645,11 +1619,11 @@
         <v>29</v>
       </c>
       <c r="B18" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A18)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A18)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C18" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A18)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A18)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D18" s="22"/>
@@ -1659,11 +1633,11 @@
         <v>30</v>
       </c>
       <c r="B19" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A19)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A19)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C19" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A19)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A19)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D19" s="22"/>
@@ -1673,11 +1647,11 @@
         <v>31</v>
       </c>
       <c r="B20" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A20)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A20)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C20" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A20)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A20)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D20" s="22"/>
@@ -1687,11 +1661,11 @@
         <v>32</v>
       </c>
       <c r="B21" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A21)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A21)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C21" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A21)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A21)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D21" s="22"/>
@@ -1701,11 +1675,11 @@
         <v>33</v>
       </c>
       <c r="B22" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A22)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A22)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C22" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A22)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A22)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D22" s="22"/>
@@ -1715,11 +1689,11 @@
         <v>34</v>
       </c>
       <c r="B23" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A23)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A23)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C23" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A23)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A23)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D23" s="21"/>
@@ -1729,11 +1703,11 @@
         <v>35</v>
       </c>
       <c r="B24" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A24)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A24)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C24" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A24)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A24)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D24" s="21"/>
@@ -1743,11 +1717,11 @@
         <v>36</v>
       </c>
       <c r="B25" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A25)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A25)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C25" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A25)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A25)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D25" s="21"/>
@@ -1757,11 +1731,11 @@
         <v>37</v>
       </c>
       <c r="B26" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A26)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A26)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C26" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A26)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A26)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D26" s="21"/>
@@ -1771,11 +1745,11 @@
         <v>38</v>
       </c>
       <c r="B27" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A27)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A27)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C27" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A27)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A27)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D27" s="21"/>
@@ -1785,11 +1759,11 @@
         <v>39</v>
       </c>
       <c r="B28" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A28)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A28)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C28" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A28)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A28)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D28" s="21"/>
@@ -1799,11 +1773,11 @@
         <v>40</v>
       </c>
       <c r="B29" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A29)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A29)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C29" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A29)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A29)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D29" s="21"/>
@@ -1813,11 +1787,11 @@
         <v>41</v>
       </c>
       <c r="B30" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A30)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A30)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C30" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A30)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A30)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D30" s="21"/>
@@ -1827,11 +1801,11 @@
         <v>42</v>
       </c>
       <c r="B31" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A31)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A31)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C31" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A31)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A31)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D31" s="21"/>
@@ -1841,11 +1815,11 @@
         <v>43</v>
       </c>
       <c r="B32" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A32)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A32)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C32" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A32)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A32)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D32" s="21"/>
@@ -1855,11 +1829,11 @@
         <v>44</v>
       </c>
       <c r="B33" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A33)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A33)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C33" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A33)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A33)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D33" s="21"/>
@@ -1869,11 +1843,11 @@
         <v>45</v>
       </c>
       <c r="B34" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A34)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A34)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C34" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A34)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A34)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D34" s="21"/>
@@ -1883,11 +1857,11 @@
         <v>46</v>
       </c>
       <c r="B35" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A35)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A35)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C35" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A35)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A35)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D35" s="23"/>
@@ -1897,11 +1871,11 @@
         <v>47</v>
       </c>
       <c r="B36" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A36)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A36)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C36" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A36)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A36)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D36" s="23"/>
@@ -1911,11 +1885,11 @@
         <v>48</v>
       </c>
       <c r="B37" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A37)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A37)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C37" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A37)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A37)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D37" s="23"/>
@@ -1925,11 +1899,11 @@
         <v>49</v>
       </c>
       <c r="B38" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A38)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A38)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C38" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A38)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A38)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D38" s="23"/>
@@ -1939,11 +1913,11 @@
         <v>50</v>
       </c>
       <c r="B39" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A39)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A39)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C39" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A39)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A39)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D39" s="23"/>
@@ -1953,11 +1927,11 @@
         <v>51</v>
       </c>
       <c r="B40" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A40)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A40)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C40" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A40)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A40)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D40" s="23"/>
@@ -1967,11 +1941,11 @@
         <v>52</v>
       </c>
       <c r="B41" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A41)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A41)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C41" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A41)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A41)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D41" s="23"/>
@@ -1981,11 +1955,11 @@
         <v>53</v>
       </c>
       <c r="B42" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A42)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A42)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C42" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A42)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A42)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D42" s="23"/>
@@ -1995,11 +1969,11 @@
         <v>54</v>
       </c>
       <c r="B43" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A43)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A43)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C43" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A43)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A43)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D43" s="26"/>
@@ -2009,11 +1983,11 @@
         <v>55</v>
       </c>
       <c r="B44" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A44)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A44)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C44" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A44)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A44)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D44" s="23"/>
@@ -2023,11 +1997,11 @@
         <v>56</v>
       </c>
       <c r="B45" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A45)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A45)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C45" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A45)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A45)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D45" s="23"/>
@@ -2037,11 +2011,11 @@
         <v>57</v>
       </c>
       <c r="B46" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A46)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A46)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C46" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A46)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A46)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D46" s="27"/>
@@ -2051,11 +2025,11 @@
         <v>58</v>
       </c>
       <c r="B47" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A47)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A47)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C47" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A47)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A47)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D47" s="23"/>
@@ -2065,11 +2039,11 @@
         <v>59</v>
       </c>
       <c r="B48" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A48)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A48)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C48" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A48)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A48)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D48" s="27"/>
@@ -2079,11 +2053,11 @@
         <v>60</v>
       </c>
       <c r="B49" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A49)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A49)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C49" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A49)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A49)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D49" s="27"/>
@@ -2093,11 +2067,11 @@
         <v>61</v>
       </c>
       <c r="B50" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A50)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A50)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C50" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A50)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A50)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D50" s="23"/>
@@ -2107,11 +2081,11 @@
         <v>62</v>
       </c>
       <c r="B51" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A51)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A51)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C51" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A51)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A51)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D51" s="27"/>
@@ -2121,11 +2095,11 @@
         <v>63</v>
       </c>
       <c r="B52" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A52)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A52)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C52" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A52)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A52)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D52" s="26"/>
@@ -2135,11 +2109,11 @@
         <v>64</v>
       </c>
       <c r="B53" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A53)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A53)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C53" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A53)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A53)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D53" s="27"/>
@@ -2149,11 +2123,11 @@
         <v>65</v>
       </c>
       <c r="B54" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A54)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A54)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C54" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A54)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A54)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D54" s="23"/>
@@ -2163,11 +2137,11 @@
         <v>66</v>
       </c>
       <c r="B55" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A55)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A55)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C55" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A55)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A55)&gt;0</f>
         <v>1</v>
       </c>
     </row>
@@ -2176,11 +2150,11 @@
         <v>67</v>
       </c>
       <c r="B56" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A56)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A56)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C56" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A56)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A56)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D56" s="27"/>
@@ -2190,11 +2164,11 @@
         <v>68</v>
       </c>
       <c r="B57" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A57)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A57)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C57" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A57)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A57)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D57" s="27"/>
@@ -2204,11 +2178,11 @@
         <v>69</v>
       </c>
       <c r="B58" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A58)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A58)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C58" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A58)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A58)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D58" s="27"/>
@@ -2218,11 +2192,11 @@
         <v>70</v>
       </c>
       <c r="B59" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A59)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A59)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C59" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A59)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A59)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D59" s="27"/>
@@ -2232,11 +2206,11 @@
         <v>71</v>
       </c>
       <c r="B60" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A60)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A60)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C60" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A60)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A60)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D60" s="27"/>
@@ -2246,11 +2220,11 @@
         <v>72</v>
       </c>
       <c r="B61" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A61)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A61)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C61" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A61)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A61)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D61" s="23"/>
@@ -2260,11 +2234,11 @@
         <v>73</v>
       </c>
       <c r="B62" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A62)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A62)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C62" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A62)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A62)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D62" s="27"/>
@@ -2274,11 +2248,11 @@
         <v>74</v>
       </c>
       <c r="B63" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A63)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A63)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C63" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A63)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A63)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D63" s="28"/>
@@ -2288,11 +2262,11 @@
         <v>75</v>
       </c>
       <c r="B64" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A64)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A64)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C64" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A64)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A64)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D64" s="23"/>
@@ -2302,11 +2276,11 @@
         <v>76</v>
       </c>
       <c r="B65" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A65)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A65)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C65" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A65)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A65)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D65" s="23"/>
@@ -2316,11 +2290,11 @@
         <v>77</v>
       </c>
       <c r="B66" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A66)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A66)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C66" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A66)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A66)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D66" s="27"/>
@@ -2330,11 +2304,11 @@
         <v>78</v>
       </c>
       <c r="B67" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A67)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A67)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C67" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A67)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A67)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D67" s="23"/>
@@ -2344,11 +2318,11 @@
         <v>79</v>
       </c>
       <c r="B68" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A68)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A68)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C68" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A68)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A68)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D68" s="23"/>
@@ -2358,11 +2332,11 @@
         <v>80</v>
       </c>
       <c r="B69" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A69)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A69)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C69" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A69)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A69)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D69" s="23"/>
@@ -2372,11 +2346,11 @@
         <v>81</v>
       </c>
       <c r="B70" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A70)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A70)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C70" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A70)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A70)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D70" s="23"/>
@@ -2386,11 +2360,11 @@
         <v>82</v>
       </c>
       <c r="B71" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A71)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A71)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C71" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A71)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A71)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D71" s="23"/>
@@ -2400,11 +2374,11 @@
         <v>83</v>
       </c>
       <c r="B72" s="24" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A72)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A72)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C72" s="24" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A72)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A72)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D72" s="27"/>
@@ -2414,11 +2388,11 @@
         <v>84</v>
       </c>
       <c r="B73" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A73)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A73)&gt;0</f>
         <v>1</v>
       </c>
       <c r="C73" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A73)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A73)&gt;0</f>
         <v>0</v>
       </c>
       <c r="D73" s="29"/>
@@ -2428,11 +2402,11 @@
         <v>85</v>
       </c>
       <c r="B74" s="16" t="b">
-        <f>COUNTIF(DAnswers!$A$2:$A$74,$A74)&gt;0</f>
+        <f>COUNTIF('Debate Answers Mean Rank'!$A$2:$A$74,$A74)&gt;0</f>
         <v>0</v>
       </c>
       <c r="C74" s="16" t="b">
-        <f>COUNTIF(Technical!$A$2:$A$74,$A74)&gt;0</f>
+        <f>COUNTIF(Practical!$A$2:$A$74,$A74)&gt;0</f>
         <v>1</v>
       </c>
       <c r="D74" s="23"/>
@@ -6523,58 +6497,58 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="32"/>
+      <c r="B1" s="9" t="s">
+        <v>86</v>
+      </c>
       <c r="C1" s="9" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="N1" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O1" s="9" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P1" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="R1" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S1" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="T1" s="9" t="s">
         <v>103</v>
       </c>
     </row>
@@ -6582,9 +6556,10 @@
       <c r="A2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B2" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="30"/>
       <c r="D2" s="30"/>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -6601,19 +6576,19 @@
       <c r="Q2" s="30"/>
       <c r="R2" s="30"/>
       <c r="S2" s="30"/>
-      <c r="T2" s="30"/>
     </row>
     <row r="3">
       <c r="A3" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="9">
+        <v>1.0</v>
+      </c>
       <c r="D3" s="9">
         <v>1.0</v>
       </c>
-      <c r="E3" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="E3" s="30"/>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
@@ -6628,18 +6603,18 @@
       <c r="Q3" s="30"/>
       <c r="R3" s="30"/>
       <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
     </row>
     <row r="4">
       <c r="A4" s="15" t="s">
         <v>16</v>
       </c>
+      <c r="B4" s="30"/>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="E4" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
@@ -6653,15 +6628,15 @@
       <c r="Q4" s="30"/>
       <c r="R4" s="30"/>
       <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
     </row>
     <row r="5">
       <c r="A5" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B5" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
@@ -6678,19 +6653,19 @@
       <c r="Q5" s="30"/>
       <c r="R5" s="30"/>
       <c r="S5" s="30"/>
-      <c r="T5" s="30"/>
     </row>
     <row r="6">
       <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
+      <c r="B6" s="30"/>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="F6" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="30"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
       <c r="J6" s="30"/>
@@ -6703,20 +6678,20 @@
       <c r="Q6" s="30"/>
       <c r="R6" s="30"/>
       <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
     </row>
     <row r="7">
       <c r="A7" s="15" t="s">
         <v>37</v>
       </c>
+      <c r="B7" s="30"/>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="G7" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="30"/>
       <c r="I7" s="30"/>
       <c r="J7" s="30"/>
       <c r="K7" s="30"/>
@@ -6728,23 +6703,23 @@
       <c r="Q7" s="30"/>
       <c r="R7" s="30"/>
       <c r="S7" s="30"/>
-      <c r="T7" s="30"/>
     </row>
     <row r="8">
       <c r="A8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="30"/>
       <c r="E8" s="30"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="H8" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="I8" s="30"/>
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
@@ -6755,12 +6730,12 @@
       <c r="Q8" s="30"/>
       <c r="R8" s="30"/>
       <c r="S8" s="30"/>
-      <c r="T8" s="30"/>
     </row>
     <row r="9">
       <c r="A9" s="15" t="s">
         <v>53</v>
       </c>
+      <c r="B9" s="30"/>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
       <c r="E9" s="30"/>
@@ -6778,12 +6753,12 @@
       <c r="Q9" s="30"/>
       <c r="R9" s="30"/>
       <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
     </row>
     <row r="10">
       <c r="A10" s="15" t="s">
         <v>18</v>
       </c>
+      <c r="B10" s="30"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>
       <c r="E10" s="30"/>
@@ -6791,13 +6766,13 @@
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
       <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="J10" s="9">
+        <v>1.0</v>
+      </c>
       <c r="K10" s="9">
         <v>1.0</v>
       </c>
-      <c r="L10" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="L10" s="30"/>
       <c r="M10" s="30"/>
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
@@ -6805,15 +6780,15 @@
       <c r="Q10" s="30"/>
       <c r="R10" s="30"/>
       <c r="S10" s="30"/>
-      <c r="T10" s="30"/>
     </row>
     <row r="11">
       <c r="A11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B11" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="30"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
       <c r="F11" s="30"/>
@@ -6830,41 +6805,41 @@
       <c r="Q11" s="30"/>
       <c r="R11" s="30"/>
       <c r="S11" s="30"/>
-      <c r="T11" s="30"/>
     </row>
     <row r="12">
       <c r="A12" s="15" t="s">
         <v>20</v>
       </c>
+      <c r="B12" s="30"/>
       <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="D12" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
       <c r="I12" s="30"/>
       <c r="J12" s="30"/>
-      <c r="K12" s="30"/>
+      <c r="K12" s="9">
+        <v>1.0</v>
+      </c>
       <c r="L12" s="9">
         <v>1.0</v>
       </c>
-      <c r="M12" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="M12" s="30"/>
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
       <c r="P12" s="30"/>
       <c r="Q12" s="30"/>
       <c r="R12" s="30"/>
       <c r="S12" s="30"/>
-      <c r="T12" s="30"/>
     </row>
     <row r="13">
       <c r="A13" s="15" t="s">
         <v>21</v>
       </c>
+      <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -6873,30 +6848,30 @@
       <c r="H13" s="30"/>
       <c r="I13" s="30"/>
       <c r="J13" s="30"/>
-      <c r="K13" s="30"/>
-      <c r="L13" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="M13" s="30"/>
-      <c r="N13" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="K13" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="L13" s="30"/>
+      <c r="M13" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="N13" s="30"/>
       <c r="O13" s="30"/>
       <c r="P13" s="30"/>
       <c r="Q13" s="30"/>
       <c r="R13" s="30"/>
       <c r="S13" s="30"/>
-      <c r="T13" s="30"/>
     </row>
     <row r="14">
       <c r="A14" s="15" t="s">
         <v>39</v>
       </c>
+      <c r="B14" s="30"/>
       <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="D14" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="30"/>
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
@@ -6911,20 +6886,20 @@
       <c r="Q14" s="30"/>
       <c r="R14" s="30"/>
       <c r="S14" s="30"/>
-      <c r="T14" s="30"/>
     </row>
     <row r="15">
       <c r="A15" s="25" t="s">
         <v>40</v>
       </c>
+      <c r="B15" s="30"/>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="G15" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="30"/>
       <c r="I15" s="30"/>
       <c r="J15" s="30"/>
       <c r="K15" s="30"/>
@@ -6936,19 +6911,19 @@
       <c r="Q15" s="30"/>
       <c r="R15" s="30"/>
       <c r="S15" s="30"/>
-      <c r="T15" s="30"/>
     </row>
     <row r="16">
       <c r="A16" s="25" t="s">
         <v>42</v>
       </c>
+      <c r="B16" s="30"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
       <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="F16" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G16" s="30"/>
       <c r="H16" s="30"/>
       <c r="I16" s="30"/>
       <c r="J16" s="30"/>
@@ -6961,12 +6936,12 @@
       <c r="Q16" s="30"/>
       <c r="R16" s="30"/>
       <c r="S16" s="30"/>
-      <c r="T16" s="30"/>
     </row>
     <row r="17">
       <c r="A17" s="25" t="s">
         <v>44</v>
       </c>
+      <c r="B17" s="30"/>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
       <c r="E17" s="30"/>
@@ -6984,17 +6959,17 @@
       <c r="Q17" s="30"/>
       <c r="R17" s="30"/>
       <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
     </row>
     <row r="18">
       <c r="A18" s="15" t="s">
         <v>51</v>
       </c>
+      <c r="B18" s="30"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="D18" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
       <c r="H18" s="30"/>
@@ -7009,17 +6984,17 @@
       <c r="Q18" s="30"/>
       <c r="R18" s="30"/>
       <c r="S18" s="30"/>
-      <c r="T18" s="30"/>
     </row>
     <row r="19">
       <c r="A19" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="B19" s="30"/>
       <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="D19" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
       <c r="H19" s="30"/>
@@ -7028,27 +7003,27 @@
       <c r="K19" s="30"/>
       <c r="L19" s="30"/>
       <c r="M19" s="30"/>
-      <c r="N19" s="30"/>
-      <c r="O19" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="N19" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="O19" s="30"/>
       <c r="P19" s="30"/>
       <c r="Q19" s="30"/>
       <c r="R19" s="30"/>
       <c r="S19" s="30"/>
-      <c r="T19" s="30"/>
     </row>
     <row r="20">
       <c r="A20" s="25" t="s">
         <v>25</v>
       </c>
+      <c r="B20" s="30"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="F20" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="G20" s="30"/>
       <c r="H20" s="30"/>
       <c r="I20" s="30"/>
       <c r="J20" s="30"/>
@@ -7061,12 +7036,12 @@
       <c r="Q20" s="30"/>
       <c r="R20" s="30"/>
       <c r="S20" s="30"/>
-      <c r="T20" s="30"/>
     </row>
     <row r="21">
       <c r="A21" s="25" t="s">
         <v>41</v>
       </c>
+      <c r="B21" s="30"/>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
       <c r="E21" s="30"/>
@@ -7077,27 +7052,27 @@
       <c r="J21" s="30"/>
       <c r="K21" s="30"/>
       <c r="L21" s="30"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="O21" s="30"/>
-      <c r="P21" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="M21" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="N21" s="30"/>
+      <c r="O21" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="P21" s="30"/>
       <c r="Q21" s="30"/>
       <c r="R21" s="30"/>
       <c r="S21" s="30"/>
-      <c r="T21" s="30"/>
     </row>
     <row r="22">
       <c r="A22" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B22" s="30"/>
+      <c r="C22" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="30"/>
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
@@ -7109,22 +7084,22 @@
       <c r="M22" s="30"/>
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="P22" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="Q22" s="30"/>
       <c r="R22" s="30"/>
       <c r="S22" s="30"/>
-      <c r="T22" s="30"/>
     </row>
     <row r="23">
       <c r="A23" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D23" s="30"/>
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
@@ -7133,54 +7108,54 @@
       <c r="J23" s="30"/>
       <c r="K23" s="30"/>
       <c r="L23" s="30"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="M23" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="N23" s="30"/>
       <c r="O23" s="30"/>
       <c r="P23" s="30"/>
       <c r="Q23" s="30"/>
       <c r="R23" s="30"/>
       <c r="S23" s="30"/>
-      <c r="T23" s="30"/>
     </row>
     <row r="24">
       <c r="A24" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D24" s="30"/>
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
       <c r="G24" s="30"/>
       <c r="H24" s="30"/>
       <c r="I24" s="30"/>
       <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="K24" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="L24" s="30"/>
       <c r="M24" s="30"/>
       <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-      <c r="P24" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="O24" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="P24" s="30"/>
       <c r="Q24" s="30"/>
       <c r="R24" s="30"/>
       <c r="S24" s="30"/>
-      <c r="T24" s="30"/>
     </row>
     <row r="25">
       <c r="A25" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
@@ -7196,20 +7171,20 @@
       <c r="Q25" s="30"/>
       <c r="R25" s="30"/>
       <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
     </row>
     <row r="26">
       <c r="A26" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B26" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C26" s="30"/>
       <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="E26" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="F26" s="30"/>
       <c r="G26" s="30"/>
       <c r="H26" s="30"/>
       <c r="I26" s="30"/>
@@ -7223,16 +7198,16 @@
       <c r="Q26" s="30"/>
       <c r="R26" s="30"/>
       <c r="S26" s="30"/>
-      <c r="T26" s="30"/>
     </row>
     <row r="27">
       <c r="A27" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D27" s="30"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
@@ -7244,18 +7219,18 @@
       <c r="M27" s="30"/>
       <c r="N27" s="30"/>
       <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="P27" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="Q27" s="30"/>
       <c r="R27" s="30"/>
       <c r="S27" s="30"/>
-      <c r="T27" s="30"/>
     </row>
     <row r="28">
       <c r="A28" s="25" t="s">
         <v>36</v>
       </c>
+      <c r="B28" s="30"/>
       <c r="C28" s="30"/>
       <c r="D28" s="30"/>
       <c r="E28" s="30"/>
@@ -7264,32 +7239,32 @@
       <c r="H28" s="30"/>
       <c r="I28" s="30"/>
       <c r="J28" s="30"/>
-      <c r="K28" s="30"/>
-      <c r="L28" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="K28" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="L28" s="30"/>
       <c r="M28" s="30"/>
       <c r="N28" s="30"/>
       <c r="O28" s="30"/>
       <c r="P28" s="30"/>
       <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="T28" s="30"/>
+      <c r="R28" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="S28" s="30"/>
     </row>
     <row r="29">
       <c r="A29" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B29" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E29" s="30"/>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
       <c r="H29" s="30"/>
@@ -7298,29 +7273,29 @@
       <c r="K29" s="30"/>
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
-      <c r="N29" s="30"/>
+      <c r="N29" s="9">
+        <v>1.0</v>
+      </c>
       <c r="O29" s="9">
         <v>1.0</v>
       </c>
       <c r="P29" s="9">
         <v>1.0</v>
       </c>
-      <c r="Q29" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="Q29" s="30"/>
       <c r="R29" s="30"/>
       <c r="S29" s="30"/>
-      <c r="T29" s="30"/>
     </row>
     <row r="30">
       <c r="A30" s="15" t="s">
         <v>49</v>
       </c>
+      <c r="B30" s="30"/>
       <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="D30" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E30" s="30"/>
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
       <c r="H30" s="30"/>
@@ -7335,12 +7310,12 @@
       <c r="Q30" s="30"/>
       <c r="R30" s="30"/>
       <c r="S30" s="30"/>
-      <c r="T30" s="30"/>
     </row>
     <row r="31">
       <c r="A31" s="25" t="s">
         <v>50</v>
       </c>
+      <c r="B31" s="30"/>
       <c r="C31" s="30"/>
       <c r="D31" s="30"/>
       <c r="E31" s="30"/>
@@ -7357,8 +7332,7 @@
       <c r="P31" s="30"/>
       <c r="Q31" s="30"/>
       <c r="R31" s="30"/>
-      <c r="S31" s="30"/>
-      <c r="T31" s="9">
+      <c r="S31" s="9">
         <v>1.0</v>
       </c>
     </row>
@@ -7366,6 +7340,7 @@
       <c r="A32" s="15" t="s">
         <v>52</v>
       </c>
+      <c r="B32" s="30"/>
       <c r="C32" s="30"/>
       <c r="D32" s="30"/>
       <c r="E32" s="30"/>
@@ -7378,19 +7353,19 @@
       <c r="L32" s="30"/>
       <c r="M32" s="30"/>
       <c r="N32" s="30"/>
-      <c r="O32" s="30"/>
-      <c r="P32" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="O32" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="P32" s="30"/>
       <c r="Q32" s="30"/>
       <c r="R32" s="30"/>
       <c r="S32" s="30"/>
-      <c r="T32" s="30"/>
     </row>
     <row r="33">
       <c r="A33" s="15" t="s">
         <v>55</v>
       </c>
+      <c r="B33" s="30"/>
       <c r="C33" s="30"/>
       <c r="D33" s="30"/>
       <c r="E33" s="30"/>
@@ -7399,10 +7374,10 @@
       <c r="H33" s="30"/>
       <c r="I33" s="30"/>
       <c r="J33" s="30"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="K33" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="L33" s="30"/>
       <c r="M33" s="30"/>
       <c r="N33" s="30"/>
       <c r="O33" s="30"/>
@@ -7410,12 +7385,12 @@
       <c r="Q33" s="30"/>
       <c r="R33" s="30"/>
       <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
     </row>
     <row r="34">
       <c r="A34" s="15" t="s">
         <v>56</v>
       </c>
+      <c r="B34" s="30"/>
       <c r="C34" s="30"/>
       <c r="D34" s="30"/>
       <c r="E34" s="30"/>
@@ -7424,25 +7399,25 @@
       <c r="H34" s="30"/>
       <c r="I34" s="30"/>
       <c r="J34" s="30"/>
-      <c r="K34" s="30"/>
-      <c r="L34" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="K34" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="L34" s="30"/>
       <c r="M34" s="30"/>
       <c r="N34" s="30"/>
-      <c r="O34" s="30"/>
-      <c r="P34" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="O34" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="P34" s="30"/>
       <c r="Q34" s="30"/>
       <c r="R34" s="30"/>
       <c r="S34" s="30"/>
-      <c r="T34" s="30"/>
     </row>
     <row r="35">
       <c r="A35" s="15" t="s">
         <v>58</v>
       </c>
+      <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="D35" s="30"/>
       <c r="E35" s="30"/>
@@ -7454,24 +7429,24 @@
       <c r="K35" s="30"/>
       <c r="L35" s="30"/>
       <c r="M35" s="30"/>
-      <c r="N35" s="30"/>
-      <c r="O35" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="N35" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="O35" s="30"/>
       <c r="P35" s="30"/>
       <c r="Q35" s="30"/>
       <c r="R35" s="30"/>
       <c r="S35" s="30"/>
-      <c r="T35" s="30"/>
     </row>
     <row r="36">
       <c r="A36" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D36" s="30"/>
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
       <c r="G36" s="30"/>
@@ -7487,12 +7462,12 @@
       <c r="Q36" s="30"/>
       <c r="R36" s="30"/>
       <c r="S36" s="30"/>
-      <c r="T36" s="30"/>
     </row>
     <row r="37">
       <c r="A37" s="15" t="s">
         <v>66</v>
       </c>
+      <c r="B37" s="30"/>
       <c r="C37" s="30"/>
       <c r="D37" s="30"/>
       <c r="E37" s="30"/>
@@ -7501,10 +7476,10 @@
       <c r="H37" s="30"/>
       <c r="I37" s="30"/>
       <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="K37" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="L37" s="30"/>
       <c r="M37" s="30"/>
       <c r="N37" s="30"/>
       <c r="O37" s="30"/>
@@ -7512,17 +7487,17 @@
       <c r="Q37" s="30"/>
       <c r="R37" s="30"/>
       <c r="S37" s="30"/>
-      <c r="T37" s="30"/>
     </row>
     <row r="38">
       <c r="A38" s="34" t="s">
         <v>72</v>
       </c>
+      <c r="B38" s="30"/>
       <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="D38" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E38" s="30"/>
       <c r="F38" s="30"/>
       <c r="G38" s="30"/>
       <c r="H38" s="30"/>
@@ -7537,12 +7512,12 @@
       <c r="Q38" s="30"/>
       <c r="R38" s="30"/>
       <c r="S38" s="30"/>
-      <c r="T38" s="30"/>
     </row>
     <row r="39">
       <c r="A39" s="33" t="s">
         <v>76</v>
       </c>
+      <c r="B39" s="30"/>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
       <c r="E39" s="30"/>
@@ -7551,10 +7526,10 @@
       <c r="H39" s="30"/>
       <c r="I39" s="30"/>
       <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="K39" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="L39" s="30"/>
       <c r="M39" s="30"/>
       <c r="N39" s="30"/>
       <c r="O39" s="30"/>
@@ -7562,17 +7537,17 @@
       <c r="Q39" s="30"/>
       <c r="R39" s="30"/>
       <c r="S39" s="30"/>
-      <c r="T39" s="30"/>
     </row>
     <row r="40">
       <c r="A40" s="34" t="s">
         <v>78</v>
       </c>
+      <c r="B40" s="30"/>
       <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="D40" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E40" s="30"/>
       <c r="F40" s="30"/>
       <c r="G40" s="30"/>
       <c r="H40" s="30"/>
@@ -7587,17 +7562,16 @@
       <c r="Q40" s="30"/>
       <c r="R40" s="30"/>
       <c r="S40" s="30"/>
-      <c r="T40" s="30"/>
     </row>
     <row r="41">
       <c r="A41" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="B41" s="30"/>
+      <c r="C41" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="D41" s="30"/>
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
@@ -7613,17 +7587,17 @@
       <c r="Q41" s="30"/>
       <c r="R41" s="30"/>
       <c r="S41" s="30"/>
-      <c r="T41" s="30"/>
     </row>
     <row r="42">
       <c r="A42" s="34" t="s">
         <v>81</v>
       </c>
+      <c r="B42" s="30"/>
       <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="D42" s="9">
+        <v>1.0</v>
+      </c>
+      <c r="E42" s="30"/>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
       <c r="H42" s="30"/>
@@ -7638,13 +7612,12 @@
       <c r="Q42" s="30"/>
       <c r="R42" s="30"/>
       <c r="S42" s="30"/>
-      <c r="T42" s="30"/>
     </row>
     <row r="43">
       <c r="A43" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="35"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="30"/>
       <c r="D43" s="30"/>
       <c r="E43" s="30"/>
@@ -7656,90 +7629,88 @@
       <c r="K43" s="30"/>
       <c r="L43" s="30"/>
       <c r="M43" s="30"/>
-      <c r="N43" s="30"/>
+      <c r="N43" s="9">
+        <v>1.0</v>
+      </c>
       <c r="O43" s="9">
         <v>1.0</v>
       </c>
-      <c r="P43" s="9">
-        <v>1.0</v>
-      </c>
+      <c r="P43" s="30"/>
       <c r="Q43" s="30"/>
       <c r="R43" s="30"/>
       <c r="S43" s="30"/>
-      <c r="T43" s="30"/>
     </row>
     <row r="44">
-      <c r="A44" s="36"/>
-      <c r="B44" s="9"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="30">
+        <f t="shared" ref="B44:S44" si="1">SUM(B2:B43)</f>
+        <v>5</v>
+      </c>
       <c r="C44" s="30">
-        <f t="shared" ref="C44:T44" si="1">SUM(C2:C43)</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="D44" s="30">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E44" s="30">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F44" s="30">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G44" s="30">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H44" s="30">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I44" s="30">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="30">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="L44" s="30">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M44" s="30">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N44" s="30">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O44" s="30">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P44" s="30">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="Q44" s="30">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R44" s="30">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S44" s="30">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="T44" s="30">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7755,9 +7726,9 @@
       <formula>"TRUE"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:T43">
+  <conditionalFormatting sqref="B2:S43">
     <cfRule type="containsBlanks" dxfId="1" priority="3">
-      <formula>LEN(TRIM(C2))=0</formula>
+      <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -7826,16 +7797,16 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="39"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="9" t="s">
         <v>107</v>
       </c>
@@ -7850,16 +7821,16 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>109</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="38">
         <v>5.0</v>
       </c>
-      <c r="D2" s="41">
+      <c r="D2" s="40">
         <f t="shared" ref="D2:D20" si="1">C2/31</f>
         <v>0.1612903226</v>
       </c>
@@ -7919,262 +7890,262 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="39" t="s">
         <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="38">
         <v>9.0</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="40">
         <f t="shared" si="1"/>
         <v>0.2903225806</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="38">
         <v>10.0</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="40">
         <f t="shared" si="1"/>
         <v>0.3225806452</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="38">
         <v>2.0</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="40">
         <f t="shared" si="1"/>
         <v>0.06451612903</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="38">
         <v>3.0</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D6" s="40">
         <f t="shared" si="1"/>
         <v>0.09677419355</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="38">
         <v>2.0</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="40">
         <f t="shared" si="1"/>
         <v>0.06451612903</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="39" t="s">
         <v>110</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C8" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="41">
+      <c r="C8" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="40">
         <f t="shared" si="1"/>
         <v>0.03225806452</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>112</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="38">
         <v>0.0</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="41">
+      <c r="C10" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="40">
         <f t="shared" si="1"/>
         <v>0.03225806452</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="38">
         <v>9.0</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D11" s="40">
         <f t="shared" si="1"/>
         <v>0.2903225806</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C12" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="D12" s="41">
+      <c r="C12" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="D12" s="40">
         <f t="shared" si="1"/>
         <v>0.03225806452</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="38">
         <v>3.0</v>
       </c>
-      <c r="D13" s="41">
+      <c r="D13" s="40">
         <f t="shared" si="1"/>
         <v>0.09677419355</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="39" t="s">
         <v>113</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="38">
         <v>4.0</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="40">
         <f t="shared" si="1"/>
         <v>0.1290322581</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="39" t="s">
         <v>112</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="38">
         <v>6.0</v>
       </c>
-      <c r="D15" s="41">
+      <c r="D15" s="40">
         <f t="shared" si="1"/>
         <v>0.1935483871</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="39" t="s">
         <v>114</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="38">
         <v>3.0</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="40">
         <f t="shared" si="1"/>
         <v>0.09677419355</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="39" t="s">
         <v>115</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="38">
         <v>0.0</v>
       </c>
-      <c r="D17" s="41">
+      <c r="D17" s="40">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="39" t="s">
         <v>111</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="D18" s="41">
+      <c r="C18" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="D18" s="40">
         <f t="shared" si="1"/>
         <v>0.03225806452</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>116</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="D19" s="41">
+      <c r="C19" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="D19" s="40">
         <f t="shared" si="1"/>
         <v>0.03225806452</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="41" t="s">
         <v>117</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -8183,22 +8154,22 @@
       <c r="C20" s="3">
         <v>1.0</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="40">
         <f t="shared" si="1"/>
         <v>0.03225806452</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="39" t="s">
         <v>122</v>
       </c>
     </row>
@@ -8206,14 +8177,14 @@
       <c r="A24" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="39">
         <f>C5+C6+C7+C10+C11+C12+C18+C2+C13</f>
         <v>27</v>
       </c>
-      <c r="D24" s="44">
+      <c r="D24" s="43">
         <f t="shared" ref="D24:D31" si="2">C24/42</f>
         <v>0.6428571429</v>
       </c>
@@ -8222,14 +8193,14 @@
       <c r="A25" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="C25" s="45">
+      <c r="C25" s="44">
         <f>C4+C8</f>
         <v>11</v>
       </c>
-      <c r="D25" s="44">
+      <c r="D25" s="43">
         <f t="shared" si="2"/>
         <v>0.2619047619</v>
       </c>
@@ -8238,14 +8209,14 @@
       <c r="A26" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="39" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="44">
         <f>C3</f>
         <v>9</v>
       </c>
-      <c r="D26" s="44">
+      <c r="D26" s="43">
         <f t="shared" si="2"/>
         <v>0.2142857143</v>
       </c>
@@ -8254,13 +8225,13 @@
       <c r="A27" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="40">
+      <c r="C27" s="39">
         <v>3.0</v>
       </c>
-      <c r="D27" s="44">
+      <c r="D27" s="43">
         <f t="shared" si="2"/>
         <v>0.07142857143</v>
       </c>
@@ -8269,13 +8240,13 @@
       <c r="A28" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="40">
+      <c r="C28" s="39">
         <v>3.0</v>
       </c>
-      <c r="D28" s="44">
+      <c r="D28" s="43">
         <f t="shared" si="2"/>
         <v>0.07142857143</v>
       </c>
@@ -8284,13 +8255,13 @@
       <c r="A29" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="39">
         <v>2.0</v>
       </c>
-      <c r="D29" s="44">
+      <c r="D29" s="43">
         <f t="shared" si="2"/>
         <v>0.04761904762</v>
       </c>
@@ -8299,13 +8270,13 @@
       <c r="A30" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="C30" s="40">
-        <v>1.0</v>
-      </c>
-      <c r="D30" s="44">
+      <c r="C30" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="D30" s="43">
         <f t="shared" si="2"/>
         <v>0.02380952381</v>
       </c>
@@ -8314,21 +8285,21 @@
       <c r="A31" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="40">
-        <v>1.0</v>
-      </c>
-      <c r="D31" s="44">
+      <c r="C31" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="D31" s="43">
         <f t="shared" si="2"/>
         <v>0.02380952381</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
-      <c r="D32" s="46"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="45"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -8359,7 +8330,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>126</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -10189,64 +10160,64 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="M1" s="47" t="s">
+      <c r="M1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="N1" s="47" t="s">
+      <c r="N1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="O1" s="47" t="s">
+      <c r="O1" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="P1" s="47" t="s">
+      <c r="P1" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="Q1" s="47" t="s">
+      <c r="Q1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="R1" s="47" t="s">
+      <c r="R1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="S1" s="47" t="s">
+      <c r="S1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="T1" s="47" t="s">
+      <c r="T1" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="U1" s="47" t="s">
+      <c r="U1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="V1" s="47" t="s">
+      <c r="V1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="W1" s="47" t="s">
+      <c r="W1" s="46" t="s">
         <v>123</v>
       </c>
       <c r="X1" s="9" t="s">
@@ -10254,7 +10225,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="35" t="s">
         <v>126</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -11309,7 +11280,7 @@
       <c r="X30" s="30"/>
     </row>
     <row r="31">
-      <c r="A31" s="48" t="s">
+      <c r="A31" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B31" s="9">
@@ -11343,7 +11314,7 @@
       <c r="X31" s="30"/>
     </row>
     <row r="32">
-      <c r="A32" s="48" t="s">
+      <c r="A32" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B32" s="9">
@@ -11379,7 +11350,7 @@
       <c r="X32" s="30"/>
     </row>
     <row r="33">
-      <c r="A33" s="48" t="s">
+      <c r="A33" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B33" s="9">
@@ -11881,7 +11852,7 @@
       <c r="X46" s="30"/>
     </row>
     <row r="47">
-      <c r="A47" s="49" t="s">
+      <c r="A47" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B47" s="9">
@@ -11916,7 +11887,7 @@
       <c r="Y47" s="30"/>
     </row>
     <row r="48">
-      <c r="A48" s="49" t="s">
+      <c r="A48" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B48" s="9">
@@ -11953,7 +11924,7 @@
       <c r="Y48" s="30"/>
     </row>
     <row r="49">
-      <c r="A49" s="49" t="s">
+      <c r="A49" s="15" t="s">
         <v>84</v>
       </c>
       <c r="B49" s="9">
@@ -11988,7 +11959,7 @@
       <c r="Y49" s="30"/>
     </row>
     <row r="50">
-      <c r="A50" s="49" t="s">
+      <c r="A50" s="15" t="s">
         <v>84</v>
       </c>
       <c r="B50" s="9">
@@ -12005,7 +11976,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="49" t="s">
+      <c r="A51" s="15" t="s">
         <v>84</v>
       </c>
       <c r="B51" s="9">
@@ -12122,7 +12093,7 @@
       <c r="C62" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D62" s="50">
+      <c r="D62" s="47">
         <f>COUNTIF(C3:C52,"=OPPOSED")</f>
         <v>19</v>
       </c>
@@ -12134,16 +12105,16 @@
         <f>MODE(B3,B6,B7,B9,B11,B13,B16,B17,B18,B19,B20,B21,B24,B25,B26,B41,B44)</f>
         <v>1</v>
       </c>
-      <c r="G62" s="51">
+      <c r="G62" s="48">
         <f>SUMIF(C3:C52, "=OPPOSED",B3:B52)</f>
         <v>36</v>
       </c>
     </row>
     <row r="63">
-      <c r="C63" s="52" t="s">
+      <c r="C63" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="D63" s="53">
+      <c r="D63" s="50">
         <f>COUNTIF(C3:C52,"=IN FAVOR")</f>
         <v>17</v>
       </c>
@@ -12155,16 +12126,16 @@
         <f>MODE(B39,B38,B35,B34,B33,B32,B31,B30,B29,B28,B27,B46,B22,B14,B12,B4,B48,B49)</f>
         <v>2</v>
       </c>
-      <c r="G63" s="51">
+      <c r="G63" s="48">
         <f>SUMIF(C3:C52, "=IN FAVOR",B3:B52)</f>
         <v>33</v>
       </c>
     </row>
     <row r="64">
-      <c r="C64" s="52" t="s">
+      <c r="C64" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="D64" s="53">
+      <c r="D64" s="50">
         <f>COUNTIF(C3:C52,"=IN FAVOR &amp; OPPOSED")</f>
         <v>12</v>
       </c>
@@ -12176,7 +12147,7 @@
         <f>MODE(B45,B43,B42,B40,B37,B36,B23,B15,B10,B8,B5,B50)</f>
         <v>2</v>
       </c>
-      <c r="G64" s="51">
+      <c r="G64" s="48">
         <f>SUMIF(C3:C52, "=IN FAVOR &amp; OPPOSED",B3:B52)</f>
         <v>22</v>
       </c>
@@ -12272,247 +12243,247 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>154</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>155</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="38">
         <v>7.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="39" t="s">
         <v>156</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="38">
         <v>10.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>157</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="38">
         <v>3.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>158</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="38">
         <v>4.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="39" t="s">
         <v>155</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="39">
+      <c r="C6" s="38">
         <v>16.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>159</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="38">
         <v>3.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="39" t="s">
         <v>160</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C8" s="39">
+      <c r="C8" s="38">
         <v>1.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="39" t="s">
         <v>161</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="38">
         <v>6.0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="39" t="s">
         <v>86</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="39">
+      <c r="C10" s="38">
         <v>4.0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>160</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="38">
         <v>0.0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="39" t="s">
         <v>158</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="39">
+      <c r="C12" s="38">
         <v>5.0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="39" t="s">
         <v>113</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="C13" s="39">
+      <c r="C13" s="38">
         <v>1.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="39" t="s">
         <v>113</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="38">
         <v>4.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="39" t="s">
         <v>158</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="38">
         <v>6.0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="39" t="s">
         <v>160</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="38">
         <v>1.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="39" t="s">
         <v>158</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="38">
         <v>1.0</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="39" t="s">
         <v>156</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C18" s="39">
+      <c r="C18" s="38">
         <v>0.0</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="39" t="s">
         <v>160</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="38">
         <v>0.0</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="39" t="s">
         <v>160</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C20" s="39">
+      <c r="C20" s="38">
         <v>7.0</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="40" t="s">
+      <c r="A21" s="39" t="s">
         <v>160</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="38">
         <v>2.0</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="40" t="s">
+      <c r="A22" s="39" t="s">
         <v>113</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C22" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="E22" s="54"/>
+      <c r="C22" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="E22" s="51"/>
     </row>
     <row r="23">
       <c r="A23" s="9" t="s">
@@ -12520,16 +12491,16 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="42" t="s">
         <v>119</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>162</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="36" t="s">
         <v>108</v>
       </c>
     </row>
@@ -12537,14 +12508,14 @@
       <c r="A25" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="C25" s="45">
+      <c r="C25" s="44">
         <f>C2+C6</f>
         <v>23</v>
       </c>
-      <c r="D25" s="44">
+      <c r="D25" s="43">
         <f t="shared" ref="D25:D32" si="1">C25/45</f>
         <v>0.5111111111</v>
       </c>
@@ -12553,14 +12524,14 @@
       <c r="A26" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="C26" s="45">
+      <c r="C26" s="44">
         <f>C5+C12+C15+C17+C4</f>
         <v>19</v>
       </c>
-      <c r="D26" s="44">
+      <c r="D26" s="43">
         <f t="shared" si="1"/>
         <v>0.4222222222</v>
       </c>
@@ -12569,14 +12540,14 @@
       <c r="A27" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="C27" s="45">
+      <c r="C27" s="44">
         <f>C21+C20+C19+C16+C11+C8</f>
         <v>11</v>
       </c>
-      <c r="D27" s="44">
+      <c r="D27" s="43">
         <f t="shared" si="1"/>
         <v>0.2444444444</v>
       </c>
@@ -12585,14 +12556,14 @@
       <c r="A28" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="C28" s="45">
+      <c r="C28" s="44">
         <f>C3+C18</f>
         <v>10</v>
       </c>
-      <c r="D28" s="44">
+      <c r="D28" s="43">
         <f t="shared" si="1"/>
         <v>0.2222222222</v>
       </c>
@@ -12601,14 +12572,14 @@
       <c r="A29" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="C29" s="40">
+      <c r="C29" s="39">
         <f>C9</f>
         <v>6</v>
       </c>
-      <c r="D29" s="44">
+      <c r="D29" s="43">
         <f t="shared" si="1"/>
         <v>0.1333333333</v>
       </c>
@@ -12617,14 +12588,14 @@
       <c r="A30" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="40">
+      <c r="C30" s="39">
         <f>C13+C14+C22</f>
         <v>6</v>
       </c>
-      <c r="D30" s="44">
+      <c r="D30" s="43">
         <f t="shared" si="1"/>
         <v>0.1333333333</v>
       </c>
@@ -12633,14 +12604,14 @@
       <c r="A31" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="C31" s="40">
+      <c r="C31" s="39">
         <f>C10</f>
         <v>4</v>
       </c>
-      <c r="D31" s="44">
+      <c r="D31" s="43">
         <f t="shared" si="1"/>
         <v>0.08888888889</v>
       </c>
@@ -12649,26 +12620,26 @@
       <c r="A32" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B32" s="40" t="s">
+      <c r="B32" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="C32" s="40">
+      <c r="C32" s="39">
         <v>3.0</v>
       </c>
-      <c r="D32" s="44">
+      <c r="D32" s="43">
         <f t="shared" si="1"/>
         <v>0.06666666667</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="55"/>
-      <c r="D33" s="56"/>
+      <c r="B33" s="52"/>
+      <c r="D33" s="53"/>
     </row>
     <row r="34">
-      <c r="D34" s="56"/>
+      <c r="D34" s="53"/>
     </row>
     <row r="35">
-      <c r="D35" s="56"/>
+      <c r="D35" s="53"/>
     </row>
     <row r="37">
       <c r="B37" s="9"/>
@@ -12697,7 +12668,7 @@
       <c r="B44" s="9"/>
     </row>
     <row r="45">
-      <c r="B45" s="55"/>
+      <c r="B45" s="52"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -12719,25 +12690,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="55" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="55" t="s">
         <v>165</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="55" t="s">
         <v>166</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="55" t="s">
         <v>169</v>
       </c>
     </row>
@@ -13051,78 +13022,78 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="37" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="B2" s="62" t="str">
+      <c r="B2" s="59" t="str">
         <f>'Debate Questions'!E1</f>
         <v>sacrificing OOP for testability / Do not want to break encapsulation for testability sake / Concern about encapsulation</v>
       </c>
-      <c r="C2" s="39">
+      <c r="C2" s="38">
         <f>'Debate Questions'!E19</f>
         <v>9</v>
       </c>
-      <c r="D2" s="41">
+      <c r="D2" s="40">
         <f t="shared" ref="D2:D5" si="1">C2/16</f>
         <v>0.5625</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="B3" s="62" t="str">
+      <c r="B3" s="59" t="str">
         <f>'Debate Questions'!D1</f>
         <v>Curiosity of why not testing non-public methods</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="38">
         <f>'Debate Questions'!D19</f>
         <v>6</v>
       </c>
-      <c r="D3" s="41">
+      <c r="D3" s="40">
         <f t="shared" si="1"/>
         <v>0.375</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="B4" s="62" t="str">
+      <c r="B4" s="59" t="str">
         <f>'Debate Questions'!B1</f>
         <v>Testing the logic / Complexity of the non-public method couldn't be handled by the public method</v>
       </c>
       <c r="C4" s="3">
         <v>5.0</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="40">
         <f t="shared" si="1"/>
         <v>0.3125</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="B5" s="62" t="str">
+      <c r="B5" s="59" t="str">
         <f>'Debate Questions'!F1</f>
         <v>Repating test if only public method is tested</v>
       </c>
       <c r="C5" s="3">
         <v>3.0</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="40">
         <f t="shared" si="1"/>
         <v>0.1875</v>
       </c>

</xml_diff>